<commit_message>
Add NCPDP Data Dictionary & Sample
</commit_message>
<xml_diff>
--- a/doc/SFDC Reference data dictionary and sample data.xlsx
+++ b/doc/SFDC Reference data dictionary and sample data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelly.xie@mckesson.com/Training/finalproject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1E0DD1-205F-E94F-BE64-24B7013982E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EA4E9-0D1F-A243-9027-71223DECFF49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26020" windowHeight="15200" activeTab="1" xr2:uid="{EA5D3A78-28CF-4141-9140-0A3F63A5D00E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26020" windowHeight="15200" activeTab="4" xr2:uid="{EA5D3A78-28CF-4141-9140-0A3F63A5D00E}"/>
   </bookViews>
   <sheets>
-    <sheet name="DRG Data" sheetId="1" r:id="rId1"/>
+    <sheet name="DRG Spec" sheetId="1" r:id="rId1"/>
     <sheet name="Payer" sheetId="3" r:id="rId2"/>
     <sheet name="Plan" sheetId="4" r:id="rId3"/>
     <sheet name="Plan State" sheetId="5" r:id="rId4"/>
+    <sheet name="NCPDP Spec" sheetId="7" r:id="rId5"/>
+    <sheet name="NCPDP" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="261">
   <si>
     <t>Payer</t>
   </si>
@@ -712,6 +714,114 @@
   </si>
   <si>
     <t>FK to Link to Payer PK to  identify the plan</t>
+  </si>
+  <si>
+    <t>NCPDP Sub Data Set</t>
+  </si>
+  <si>
+    <t>PHARMACY_ID</t>
+  </si>
+  <si>
+    <t>PHARMACY_NAME</t>
+  </si>
+  <si>
+    <t>NCPDP</t>
+  </si>
+  <si>
+    <t>NPI_NBR</t>
+  </si>
+  <si>
+    <t>PHONE_NBR</t>
+  </si>
+  <si>
+    <t>FAX_NBR</t>
+  </si>
+  <si>
+    <t>UK for a given Pharmacy, NCPDP Number</t>
+  </si>
+  <si>
+    <t>NPI Number</t>
+  </si>
+  <si>
+    <t>Pharmacy Phone</t>
+  </si>
+  <si>
+    <t>Pharmacy Fax</t>
+  </si>
+  <si>
+    <t>Pharmacy</t>
+  </si>
+  <si>
+    <t>WALGREENS</t>
+  </si>
+  <si>
+    <t>US BIOSERVICES</t>
+  </si>
+  <si>
+    <t>ACCREDO</t>
+  </si>
+  <si>
+    <t>AET</t>
+  </si>
+  <si>
+    <t>BIOSCRIP</t>
+  </si>
+  <si>
+    <t>CAREMARK</t>
+  </si>
+  <si>
+    <t>CAREPLUS</t>
+  </si>
+  <si>
+    <t>CIGNA</t>
+  </si>
+  <si>
+    <t>CURASCRIPT SPECIALTY PHARMACY</t>
+  </si>
+  <si>
+    <t>ICORE HEALTHCARE SPECIALTY PHARMACY</t>
+  </si>
+  <si>
+    <t>HUMANA RS SPECIALTY PHARMACY</t>
+  </si>
+  <si>
+    <t>PRESCRIPTION SOLUTIONS SPECIALT PHARMACY</t>
+  </si>
+  <si>
+    <t>WALGREENS SPECIALTY PHARMACY</t>
+  </si>
+  <si>
+    <t>MEDVANTX</t>
+  </si>
+  <si>
+    <t>APOTHECARY</t>
+  </si>
+  <si>
+    <t>COMMCARE</t>
+  </si>
+  <si>
+    <t>MODERN</t>
+  </si>
+  <si>
+    <t>ABC PHARMACY</t>
+  </si>
+  <si>
+    <t>AVELLA</t>
+  </si>
+  <si>
+    <t>MCKESSON SPECIALTY PHARMACY</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>ACARIAHEALTH PHARMACY #11 INC</t>
+  </si>
+  <si>
+    <t>ACRO PHARMACEUTICAL SERVICES</t>
+  </si>
+  <si>
+    <t>ACS</t>
   </si>
 </sst>
 </file>
@@ -814,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -836,6 +946,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,7 +1267,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1372,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8F5A7A-800E-4A54-A28B-F5CCF6CDC1E0}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -10031,19 +10144,678 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E952AA-F3DE-8C4A-815E-F12DC71FF1B0}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="34" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37557F49-F0BA-C445-98FD-49F51B058B59}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>14256</v>
+      </c>
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2">
+        <v>32079</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>14259</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3">
+        <v>453180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>14260</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4">
+        <v>453180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>14262</v>
+      </c>
+      <c r="B5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5">
+        <v>32079</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>14265</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6">
+        <v>9876123</v>
+      </c>
+      <c r="D6">
+        <v>9939911111</v>
+      </c>
+      <c r="E6">
+        <v>9919991112</v>
+      </c>
+      <c r="F6">
+        <v>8818828881</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14266</v>
+      </c>
+      <c r="B7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7">
+        <v>2342342</v>
+      </c>
+      <c r="D7">
+        <v>3243242343</v>
+      </c>
+      <c r="E7">
+        <v>9939919922</v>
+      </c>
+      <c r="F7">
+        <v>2342343242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>14267</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8">
+        <v>2342343</v>
+      </c>
+      <c r="D8">
+        <v>3243243242</v>
+      </c>
+      <c r="E8">
+        <v>2231113334</v>
+      </c>
+      <c r="F8">
+        <v>1221331112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>14268</v>
+      </c>
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9">
+        <v>2132132</v>
+      </c>
+      <c r="D9">
+        <v>3434534543</v>
+      </c>
+      <c r="E9">
+        <v>1223331112</v>
+      </c>
+      <c r="F9">
+        <v>1231231231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10">
+        <v>9213123</v>
+      </c>
+      <c r="D10">
+        <v>2132131232</v>
+      </c>
+      <c r="E10">
+        <v>9919929911</v>
+      </c>
+      <c r="F10">
+        <v>9919393111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14270</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11">
+        <v>2332432</v>
+      </c>
+      <c r="D11">
+        <v>2342343243</v>
+      </c>
+      <c r="E11">
+        <v>2132221111</v>
+      </c>
+      <c r="F11">
+        <v>2223331111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>14271</v>
+      </c>
+      <c r="B12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12">
+        <v>4567257</v>
+      </c>
+      <c r="E12">
+        <v>6027038628</v>
+      </c>
+      <c r="F12">
+        <v>2052534911</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>14272</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13">
+        <v>8888888</v>
+      </c>
+      <c r="E13">
+        <v>6027038628</v>
+      </c>
+      <c r="F13">
+        <v>2052534900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14273</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14">
+        <v>9999999</v>
+      </c>
+      <c r="E14">
+        <v>6027038628</v>
+      </c>
+      <c r="F14">
+        <v>2052534900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14274</v>
+      </c>
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15">
+        <v>1010101</v>
+      </c>
+      <c r="E15">
+        <v>6027038628</v>
+      </c>
+      <c r="F15">
+        <v>2052534900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14275</v>
+      </c>
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16">
+        <v>1111111</v>
+      </c>
+      <c r="E16">
+        <v>6027038628</v>
+      </c>
+      <c r="F16">
+        <v>2052534900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>14279</v>
+      </c>
+      <c r="B17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17">
+        <v>435196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14280</v>
+      </c>
+      <c r="B18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18">
+        <v>1111119</v>
+      </c>
+      <c r="E18">
+        <v>6027038628</v>
+      </c>
+      <c r="F18">
+        <v>2083610545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14281</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C19">
+        <v>1122334</v>
+      </c>
+      <c r="E19">
+        <v>6027038628</v>
+      </c>
+      <c r="F19">
+        <v>2083610545</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>14282</v>
+      </c>
+      <c r="B20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C20">
+        <v>5556667</v>
+      </c>
+      <c r="E20">
+        <v>2052534911</v>
+      </c>
+      <c r="F20">
+        <v>2052534900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>14283</v>
+      </c>
+      <c r="B21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21">
+        <v>1146693</v>
+      </c>
+      <c r="E21">
+        <v>4048929131</v>
+      </c>
+      <c r="F21">
+        <v>4048928102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>14285</v>
+      </c>
+      <c r="B22" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22">
+        <v>4675896</v>
+      </c>
+      <c r="D22">
+        <v>9578346934</v>
+      </c>
+      <c r="E22">
+        <v>9876543210</v>
+      </c>
+      <c r="F22">
+        <v>9876543210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>14286</v>
+      </c>
+      <c r="B23" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23">
+        <v>354643</v>
+      </c>
+      <c r="E23">
+        <v>4444444444</v>
+      </c>
+      <c r="F23">
+        <v>5555555555</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>14297</v>
+      </c>
+      <c r="B24" t="s">
+        <v>256</v>
+      </c>
+      <c r="C24">
+        <v>35271</v>
+      </c>
+      <c r="D24">
+        <v>1205035011</v>
+      </c>
+      <c r="E24">
+        <v>4806634160</v>
+      </c>
+      <c r="F24">
+        <v>8665583777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>14298</v>
+      </c>
+      <c r="B25" t="s">
+        <v>257</v>
+      </c>
+      <c r="C25">
+        <v>1212132</v>
+      </c>
+      <c r="E25">
+        <v>1234567890</v>
+      </c>
+      <c r="F25">
+        <v>9999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>14305</v>
+      </c>
+      <c r="B26" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26">
+        <v>35271</v>
+      </c>
+      <c r="D26">
+        <v>1205035011</v>
+      </c>
+      <c r="E26">
+        <v>4806634160</v>
+      </c>
+      <c r="F26">
+        <v>8665583777</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>14306</v>
+      </c>
+      <c r="B27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C27">
+        <v>4544424</v>
+      </c>
+      <c r="D27">
+        <v>1629195045</v>
+      </c>
+      <c r="E27">
+        <v>7136518001</v>
+      </c>
+      <c r="F27">
+        <v>8775411503</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14307</v>
+      </c>
+      <c r="B28" t="s">
+        <v>259</v>
+      </c>
+      <c r="C28">
+        <v>1111111</v>
+      </c>
+      <c r="D28">
+        <v>1639103823</v>
+      </c>
+      <c r="E28">
+        <v>8009067798</v>
+      </c>
+      <c r="F28">
+        <v>4844948235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>14308</v>
+      </c>
+      <c r="B29" t="s">
+        <v>260</v>
+      </c>
+      <c r="C29">
+        <v>1013438</v>
+      </c>
+      <c r="D29">
+        <v>1063510097</v>
+      </c>
+      <c r="E29">
+        <v>8779856337</v>
+      </c>
+      <c r="F29">
+        <v>8773813806</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>14309</v>
+      </c>
+      <c r="B30" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30">
+        <v>2222222</v>
+      </c>
+      <c r="D30">
+        <v>1275532053</v>
+      </c>
+      <c r="E30">
+        <v>8885187246</v>
+      </c>
+      <c r="F30">
+        <v>8778172965</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10264,6 +11036,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B013CE4-9A04-430D-964F-80ED3A29FE70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68F03921-F0D9-481D-9ADE-AA13076A4B98}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -10276,14 +11056,6 @@
     <ds:schemaRef ds:uri="408e6010-c483-496d-8546-1cd7fdc08bdd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B013CE4-9A04-430D-964F-80ED3A29FE70}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
file cleanup before merge to master
</commit_message>
<xml_diff>
--- a/doc/SFDC Reference data dictionary and sample data.xlsx
+++ b/doc/SFDC Reference data dictionary and sample data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelly.xie@mckesson.com/Training/finalproject/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EA4E9-0D1F-A243-9027-71223DECFF49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41455596-64B4-4249-9510-2738F45FCC90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26020" windowHeight="15200" activeTab="4" xr2:uid="{EA5D3A78-28CF-4141-9140-0A3F63A5D00E}"/>
+    <workbookView xWindow="7520" yWindow="3760" windowWidth="26020" windowHeight="15200" activeTab="5" xr2:uid="{EA5D3A78-28CF-4141-9140-0A3F63A5D00E}"/>
   </bookViews>
   <sheets>
     <sheet name="DRG Spec" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="268">
   <si>
     <t>Payer</t>
   </si>
@@ -822,6 +822,27 @@
   </si>
   <si>
     <t>ACS</t>
+  </si>
+  <si>
+    <t>File Format</t>
+  </si>
+  <si>
+    <t>File format</t>
+  </si>
+  <si>
+    <t>comma delimitor</t>
+  </si>
+  <si>
+    <t>*.csv</t>
+  </si>
+  <si>
+    <t>*.txt</t>
+  </si>
+  <si>
+    <t>pipe Delimitor</t>
+  </si>
+  <si>
+    <t>Parent Id</t>
   </si>
 </sst>
 </file>
@@ -924,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -946,6 +967,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1264,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB5924D-159D-488C-B592-5669A3B6CE5A}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1468,6 +1492,17 @@
       </c>
       <c r="C22" s="2" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1483,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8F5A7A-800E-4A54-A28B-F5CCF6CDC1E0}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1495,15 +1530,18 @@
     <col min="2" max="2" width="53.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>141</v>
       </c>
@@ -1511,7 +1549,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1487</v>
       </c>
@@ -1519,7 +1557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2890</v>
       </c>
@@ -1527,7 +1565,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>842</v>
       </c>
@@ -1535,7 +1573,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>3257</v>
       </c>
@@ -1543,7 +1581,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>2690</v>
       </c>
@@ -1551,7 +1589,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>1489</v>
       </c>
@@ -1559,7 +1597,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>2684</v>
       </c>
@@ -1567,7 +1605,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>2681</v>
       </c>
@@ -1575,7 +1613,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>2668</v>
       </c>
@@ -1583,7 +1621,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>2663</v>
       </c>
@@ -1591,7 +1629,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>1491</v>
       </c>
@@ -1599,7 +1637,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>2558</v>
       </c>
@@ -1607,7 +1645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>904</v>
       </c>
@@ -1615,7 +1653,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>140</v>
       </c>
@@ -3005,7 +3043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F77A06-23AE-4312-AF09-E65848016DFC}">
   <dimension ref="A1:B891"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -10146,15 +10184,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E952AA-F3DE-8C4A-815E-F12DC71FF1B0}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
@@ -10214,7 +10252,7 @@
       <c r="B7" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>232</v>
       </c>
     </row>
@@ -10225,7 +10263,7 @@
       <c r="B8" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>233</v>
       </c>
     </row>
@@ -10236,7 +10274,7 @@
       <c r="B9" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>234</v>
       </c>
     </row>
@@ -10247,8 +10285,19 @@
       <c r="B10" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -10264,7 +10313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37557F49-F0BA-C445-98FD-49F51B058B59}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>